<commit_message>
Second pass is working, gloriously able to correctly identify ALL tables 	in he test dataset
</commit_message>
<xml_diff>
--- a/out/AC/AC 1424.xlsx
+++ b/out/AC/AC 1424.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Kundenr</t>
   </si>
@@ -380,7 +380,7 @@
     <t>5% filler,10% containsTotalMass,10% containsSingleMass,52% isInteger,10% containsProductNr,10% containsAmount,</t>
   </si>
   <si>
-    <t>4% filler,23% containsTotalMass,23% containsSingleMass,47% isDecimal,</t>
+    <t>4% filler,22% containsTotalMass,22% containsSingleMass,45% isDecimal,4% containsAmount,</t>
   </si>
   <si>
     <t>4% filler,47% containsProduct,47% QuantityHeader,</t>
@@ -407,7 +407,7 @@
     <t>4% filler,47% containsProduct,47% SingleMassHeader,</t>
   </si>
   <si>
-    <t>6% filler,31% containsProductNr,62% containsAmount,</t>
+    <t>3% filler,38% containsProduct,19% containsProductNr,38% containsAmount,</t>
   </si>
   <si>
     <t>2% filler,27% containsProduct,13% containsProductNr,27% containsAmount,27% QuantityHeader,</t>
@@ -419,16 +419,13 @@
     <t>3% filler,32% containsProduct,32% containsProductNr,32% containsAmount,</t>
   </si>
   <si>
+    <t>6% filler,31% containsProductNr,62% containsAmount,</t>
+  </si>
+  <si>
     <t>1% filler,15% containsTotalMass,15% containsSingleMass,15% containsProduct,7% containsProductNr,15% containsAmount,15% SingleMassHeader,15% TotalMassHeader,</t>
   </si>
   <si>
-    <t>3% filler,38% containsProduct,19% containsProductNr,38% containsAmount,</t>
-  </si>
-  <si>
     <t>1% filler,19% containsTotalMass,19% containsSingleMass,19% containsProduct,19% SingleMassHeader,19% TotalMassHeader,</t>
-  </si>
-  <si>
-    <t>1% filler,17% containsTotalMass,17% containsSingleMass,8% containsProductNr,17% containsAmount,17% SingleMassHeader,17% TotalMassHeader,</t>
   </si>
   <si>
     <t xml:space="preserve">VARENR, </t>
@@ -438,6 +435,12 @@
   </si>
   <si>
     <t xml:space="preserve">PRODUKT, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANTAL, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">STK. MASSE, TOTAL MASSE </t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="61">
+  <fills count="60">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,7 +801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE3DD42"/>
+        <fgColor rgb="FFD8D34A"/>
       </patternFill>
     </fill>
     <fill>
@@ -843,7 +846,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0F08A6"/>
+        <fgColor rgb="FF093666"/>
       </patternFill>
     </fill>
     <fill>
@@ -863,22 +866,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF0F08A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF8C898B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF093666"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB6B281"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA58BA3"/>
       </patternFill>
     </fill>
     <fill>
@@ -1062,7 +1060,7 @@
     <xf numFmtId="0" applyNumberFormat="0" fontId="16" applyFont="1" fillId="0" applyFill="0" borderId="9" applyBorder="1" applyProtection="0" applyAlignment="0"/>
     <xf numFmtId="0" applyNumberFormat="0" fontId="7" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" applyFont="1" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" applyNumberFormat="1" fontId="16" applyFont="1" fillId="0" borderId="0" xfId="0"/>
@@ -1096,15 +1094,14 @@
     <xf numFmtId="0" fontId="0" fillId="50" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="51" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="52" applyFill="1" borderId="0"/>
-    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="49" applyFill="1" borderId="0" xfId="0"/>
+    <xf numFmtId="2" applyNumberFormat="1" fontId="0" fillId="53" applyFill="1" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="53" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="54" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="55" applyFill="1" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="56" applyFill="1" borderId="0"/>
+    <xf numFmtId="0" fontId="16" applyFont="1" fillId="56" applyFill="1" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" applyFont="1" fillId="57" applyFill="1" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" applyFont="1" fillId="58" applyFill="1" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="58" applyFill="1" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="59" applyFill="1" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="60" applyFill="1" borderId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Farve1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -10364,9 +10361,6 @@
         <f t="shared" si="0"/>
         <v>185</v>
       </c>
-      <c r="I24" s="37" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="17">
@@ -11242,7 +11236,7 @@
       <c r="C57" s="17">
         <v>921050</v>
       </c>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="35" t="s">
         <v>64</v>
       </c>
       <c r="E57" s="17">
@@ -11404,7 +11398,7 @@
       <c r="C63" s="17">
         <v>921500</v>
       </c>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E63" s="18">
@@ -11755,7 +11749,7 @@
       <c r="C76" s="17">
         <v>924820</v>
       </c>
-      <c r="D76" s="35" t="s">
+      <c r="D76" s="29" t="s">
         <v>83</v>
       </c>
       <c r="E76" s="17">
@@ -11809,7 +11803,7 @@
       <c r="C78" s="17">
         <v>925400</v>
       </c>
-      <c r="D78" s="34" t="s">
+      <c r="D78" s="35" t="s">
         <v>85</v>
       </c>
       <c r="E78" s="17">
@@ -11998,7 +11992,7 @@
       <c r="C85" s="17">
         <v>926340</v>
       </c>
-      <c r="D85" s="37" t="s">
+      <c r="D85" s="35" t="s">
         <v>92</v>
       </c>
       <c r="E85" s="17">
@@ -12079,7 +12073,7 @@
       <c r="C88" s="17">
         <v>928700</v>
       </c>
-      <c r="D88" s="35" t="s">
+      <c r="D88" s="29" t="s">
         <v>95</v>
       </c>
       <c r="E88" s="18">
@@ -12106,7 +12100,7 @@
       <c r="C89" s="17">
         <v>928720</v>
       </c>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="35" t="s">
         <v>96</v>
       </c>
       <c r="E89" s="17">
@@ -12133,7 +12127,7 @@
       <c r="C90" s="17">
         <v>928800</v>
       </c>
-      <c r="D90" s="34" t="s">
+      <c r="D90" s="35" t="s">
         <v>97</v>
       </c>
       <c r="E90" s="17">
@@ -12376,7 +12370,7 @@
       <c r="C99" s="17">
         <v>933800</v>
       </c>
-      <c r="D99" s="35" t="s">
+      <c r="D99" s="29" t="s">
         <v>106</v>
       </c>
       <c r="E99" s="17">
@@ -12430,7 +12424,7 @@
       <c r="C101" s="17">
         <v>935100</v>
       </c>
-      <c r="D101" s="35" t="s">
+      <c r="D101" s="29" t="s">
         <v>108</v>
       </c>
       <c r="E101" s="17">
@@ -12511,7 +12505,7 @@
       <c r="C104" s="17">
         <v>977500</v>
       </c>
-      <c r="D104" s="34" t="s">
+      <c r="D104" s="35" t="s">
         <v>111</v>
       </c>
       <c r="E104" s="17">
@@ -17929,23 +17923,23 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="F1" s="38" t="s">
+        <v>139</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -17955,22 +17949,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="40">
+      <c r="A2" s="39">
         <v>1424</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="39">
         <v>10540</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0">
+      <c r="E2" s="39">
         <v>3.1</v>
       </c>
-      <c r="F2" s="0">
+      <c r="F2" s="40">
         <v>14</v>
       </c>
       <c r="G2" s="0">
@@ -17982,22 +17976,22 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="40">
+      <c r="A3" s="39">
         <v>1424</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="39">
         <v>13910</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0">
+      <c r="E3" s="39">
         <v>0.82</v>
       </c>
-      <c r="F3" s="0">
+      <c r="F3" s="40">
         <v>4.38</v>
       </c>
       <c r="G3" s="0">
@@ -18009,22 +18003,22 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="40">
+      <c r="A4" s="39">
         <v>1424</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="39">
         <v>13930</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4" s="39">
         <v>2.2</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4" s="40">
         <v>22</v>
       </c>
       <c r="G4" s="0">
@@ -18036,22 +18030,22 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="40">
+      <c r="A5" s="39">
         <v>1424</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="39">
         <v>13940</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5" s="39">
         <v>43.33</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5" s="40">
         <v>229.199</v>
       </c>
       <c r="G5" s="0">
@@ -18063,22 +18057,22 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="40">
+      <c r="A6" s="39">
         <v>1424</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="39">
         <v>14720</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6" s="39">
         <v>1.14</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6" s="40">
         <v>11.39</v>
       </c>
       <c r="G6" s="0">
@@ -18090,22 +18084,22 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="40">
+      <c r="A7" s="39">
         <v>1424</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="39">
         <v>21080</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7" s="39">
         <v>1</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7" s="40">
         <v>6</v>
       </c>
       <c r="G7" s="0">
@@ -18117,22 +18111,22 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="40">
+      <c r="A8" s="39">
         <v>1424</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="39">
         <v>24260</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8" s="39">
         <v>0.08</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8" s="40">
         <v>0.184</v>
       </c>
       <c r="G8" s="0">
@@ -18144,22 +18138,22 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="40">
+      <c r="A9" s="39">
         <v>1424</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="39">
         <v>24810</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9" s="39">
         <v>3.5</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9" s="40">
         <v>10.5</v>
       </c>
       <c r="G9" s="0">
@@ -18171,22 +18165,22 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="40">
+      <c r="A10" s="39">
         <v>1424</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="39">
         <v>24820</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10" s="39">
         <v>9.8</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10" s="40">
         <v>24.5</v>
       </c>
       <c r="G10" s="0">
@@ -18198,22 +18192,22 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="40">
+      <c r="A11" s="39">
         <v>1424</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <v>24840</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11" s="39">
         <v>0.4</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11" s="40">
         <v>1.2</v>
       </c>
       <c r="G11" s="0">
@@ -18225,22 +18219,22 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="40">
+      <c r="A12" s="39">
         <v>1424</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="39">
         <v>25300</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12" s="39">
         <v>6.6</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12" s="40">
         <v>33</v>
       </c>
       <c r="G12" s="0">
@@ -18252,22 +18246,22 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="40">
+      <c r="A13" s="39">
         <v>1424</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="39">
         <v>25400</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13" s="39">
         <v>3</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13" s="40">
         <v>18</v>
       </c>
       <c r="G13" s="0">
@@ -18279,22 +18273,22 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="40">
+      <c r="A14" s="39">
         <v>1424</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="39">
         <v>25710</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="0">
+      <c r="E14" s="39">
         <v>3</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14" s="40">
         <v>3</v>
       </c>
       <c r="G14" s="0">
@@ -18306,22 +18300,22 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15" s="39">
         <v>1424</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="0">
+      <c r="C15" s="39">
         <v>26230</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="0">
+      <c r="E15" s="39">
         <v>3</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15" s="40">
         <v>4.5</v>
       </c>
       <c r="G15" s="0">
@@ -18333,22 +18327,22 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16" s="39">
         <v>1424</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="0">
+      <c r="C16" s="39">
         <v>28700</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="0">
+      <c r="E16" s="39">
         <v>3</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16" s="40">
         <v>5.4</v>
       </c>
       <c r="G16" s="0">
@@ -18360,22 +18354,22 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17" s="39">
         <v>1424</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="0">
+      <c r="C17" s="39">
         <v>32990</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="0">
+      <c r="E17" s="39">
         <v>20</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17" s="40">
         <v>20</v>
       </c>
       <c r="G17" s="0">
@@ -18387,22 +18381,22 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18" s="39">
         <v>1424</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="0">
+      <c r="C18" s="39">
         <v>33520</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="0">
+      <c r="E18" s="39">
         <v>20</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18" s="40">
         <v>100</v>
       </c>
       <c r="G18" s="0">
@@ -18414,22 +18408,22 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19" s="39">
         <v>1424</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C19" s="39">
         <v>33830</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E19" s="39">
         <v>1</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19" s="40">
         <v>5</v>
       </c>
       <c r="G19" s="0">
@@ -18441,22 +18435,22 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20" s="39">
         <v>1424</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="0">
+      <c r="C20" s="39">
         <v>45600</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="0">
+      <c r="E20" s="39">
         <v>1</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20" s="40">
         <v>6</v>
       </c>
       <c r="G20" s="0">
@@ -18468,22 +18462,22 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21" s="39">
         <v>1424</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="0">
+      <c r="C21" s="39">
         <v>72200</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="0">
+      <c r="E21" s="39">
         <v>126</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21" s="40">
         <v>18.9</v>
       </c>
       <c r="G21" s="0">
@@ -18495,22 +18489,22 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22" s="39">
         <v>1424</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="0">
+      <c r="C22" s="39">
         <v>74410</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="0">
+      <c r="E22" s="39">
         <v>103</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22" s="40">
         <v>20.6</v>
       </c>
       <c r="G22" s="0">
@@ -18522,22 +18516,22 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23" s="39">
         <v>1424</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="0">
+      <c r="C23" s="39">
         <v>76800</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="0">
+      <c r="E23" s="39">
         <v>154</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23" s="40">
         <v>15.4</v>
       </c>
       <c r="G23" s="0">
@@ -18549,22 +18543,22 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24" s="39">
         <v>1424</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="0">
+      <c r="C24" s="39">
         <v>76820</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="0">
+      <c r="E24" s="39">
         <v>5</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24" s="40">
         <v>5</v>
       </c>
       <c r="G24" s="0">
@@ -18576,22 +18570,22 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25" s="39">
         <v>1424</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="0">
+      <c r="C25" s="39">
         <v>79500</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="0">
+      <c r="E25" s="39">
         <v>4</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25" s="40">
         <v>0.3</v>
       </c>
       <c r="G25" s="0">
@@ -18603,22 +18597,22 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26" s="39">
         <v>1424</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26" s="39">
         <v>79540</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="0">
+      <c r="E26" s="39">
         <v>89</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26" s="40">
         <v>6.675</v>
       </c>
       <c r="G26" s="0">
@@ -18630,22 +18624,22 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="0">
+      <c r="A27" s="39">
         <v>1424</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27" s="39">
         <v>79550</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="0">
+      <c r="E27" s="39">
         <v>41</v>
       </c>
-      <c r="F27" s="0">
+      <c r="F27" s="40">
         <v>3.075</v>
       </c>
       <c r="G27" s="0">
@@ -18657,22 +18651,22 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="0">
+      <c r="A28" s="39">
         <v>1424</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="0">
+      <c r="C28" s="39">
         <v>79560</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="0">
+      <c r="E28" s="39">
         <v>2</v>
       </c>
-      <c r="F28" s="0">
+      <c r="F28" s="40">
         <v>0.15</v>
       </c>
       <c r="G28" s="0">
@@ -18684,22 +18678,22 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="0">
+      <c r="A29" s="39">
         <v>1424</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="0">
+      <c r="C29" s="39">
         <v>79570</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="0">
+      <c r="E29" s="39">
         <v>25</v>
       </c>
-      <c r="F29" s="0">
+      <c r="F29" s="40">
         <v>1.875</v>
       </c>
       <c r="G29" s="0">
@@ -18711,22 +18705,22 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="0">
+      <c r="A30" s="39">
         <v>1424</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="0">
+      <c r="C30" s="39">
         <v>79580</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="0">
+      <c r="E30" s="39">
         <v>7</v>
       </c>
-      <c r="F30" s="0">
+      <c r="F30" s="40">
         <v>0.525</v>
       </c>
       <c r="G30" s="0">
@@ -18738,22 +18732,22 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="0">
+      <c r="A31" s="39">
         <v>1424</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="0">
+      <c r="C31" s="39">
         <v>79590</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="0">
+      <c r="E31" s="39">
         <v>3</v>
       </c>
-      <c r="F31" s="0">
+      <c r="F31" s="40">
         <v>0.225</v>
       </c>
       <c r="G31" s="0">
@@ -18765,22 +18759,22 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="0">
+      <c r="A32" s="39">
         <v>1424</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="0">
+      <c r="C32" s="39">
         <v>79610</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="0">
+      <c r="E32" s="39">
         <v>59</v>
       </c>
-      <c r="F32" s="0">
+      <c r="F32" s="40">
         <v>4.425</v>
       </c>
       <c r="G32" s="0">
@@ -18792,22 +18786,22 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="0">
+      <c r="A33" s="39">
         <v>1424</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="0">
+      <c r="C33" s="39">
         <v>79630</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="0">
+      <c r="E33" s="39">
         <v>13</v>
       </c>
-      <c r="F33" s="0">
+      <c r="F33" s="40">
         <v>0.975</v>
       </c>
       <c r="G33" s="0">
@@ -18819,22 +18813,22 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="0">
+      <c r="A34" s="39">
         <v>1424</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="0">
+      <c r="C34" s="39">
         <v>79660</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="0">
+      <c r="E34" s="39">
         <v>50</v>
       </c>
-      <c r="F34" s="0">
+      <c r="F34" s="40">
         <v>3.75</v>
       </c>
       <c r="G34" s="0">
@@ -18846,22 +18840,22 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="0">
+      <c r="A35" s="39">
         <v>1424</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="0">
+      <c r="C35" s="39">
         <v>79670</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E35" s="0">
+      <c r="E35" s="39">
         <v>1</v>
       </c>
-      <c r="F35" s="0">
+      <c r="F35" s="40">
         <v>1</v>
       </c>
       <c r="G35" s="0">
@@ -18873,22 +18867,22 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="0">
+      <c r="A36" s="39">
         <v>1424</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="0">
+      <c r="C36" s="39">
         <v>79740</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="0">
+      <c r="E36" s="39">
         <v>1</v>
       </c>
-      <c r="F36" s="0">
+      <c r="F36" s="40">
         <v>1</v>
       </c>
       <c r="G36" s="0">
@@ -18900,22 +18894,22 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="0">
+      <c r="A37" s="39">
         <v>1424</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="0">
+      <c r="C37" s="39">
         <v>79760</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="0">
+      <c r="E37" s="39">
         <v>1</v>
       </c>
-      <c r="F37" s="0">
+      <c r="F37" s="40">
         <v>1</v>
       </c>
       <c r="G37" s="0">
@@ -18927,22 +18921,22 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="0">
+      <c r="A38" s="39">
         <v>1424</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="0">
+      <c r="C38" s="39">
         <v>79810</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="0">
+      <c r="E38" s="39">
         <v>1</v>
       </c>
-      <c r="F38" s="0">
+      <c r="F38" s="40">
         <v>1</v>
       </c>
       <c r="G38" s="0">
@@ -18954,22 +18948,22 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="0">
+      <c r="A39" s="39">
         <v>1424</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="0">
+      <c r="C39" s="39">
         <v>88300</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="0">
+      <c r="E39" s="39">
         <v>0.33</v>
       </c>
-      <c r="F39" s="0">
+      <c r="F39" s="40">
         <v>0.5</v>
       </c>
       <c r="G39" s="0">
@@ -18981,22 +18975,22 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="0">
+      <c r="A40" s="39">
         <v>1424</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="0">
+      <c r="C40" s="39">
         <v>700100</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="E40" s="0">
+      <c r="E40" s="39">
         <v>1</v>
       </c>
-      <c r="F40" s="0">
+      <c r="F40" s="40">
         <v>0</v>
       </c>
       <c r="G40" s="0">
@@ -19008,22 +19002,22 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="0">
+      <c r="A41" s="39">
         <v>1424</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C41" s="0">
+      <c r="C41" s="39">
         <v>910200</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="E41" s="0">
+      <c r="E41" s="39">
         <v>26</v>
       </c>
-      <c r="F41" s="0">
+      <c r="F41" s="40">
         <v>489.32</v>
       </c>
       <c r="G41" s="0">
@@ -19035,22 +19029,22 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="0">
+      <c r="A42" s="39">
         <v>1424</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="0">
+      <c r="C42" s="39">
         <v>910210</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="0">
+      <c r="E42" s="39">
         <v>85</v>
       </c>
-      <c r="F42" s="0">
+      <c r="F42" s="40">
         <v>1156</v>
       </c>
       <c r="G42" s="0">
@@ -19062,22 +19056,22 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="0">
+      <c r="A43" s="39">
         <v>1424</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="0">
+      <c r="C43" s="39">
         <v>910440</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="0">
+      <c r="E43" s="39">
         <v>0.22</v>
       </c>
-      <c r="F43" s="0">
+      <c r="F43" s="40">
         <v>1.3</v>
       </c>
       <c r="G43" s="0">
@@ -19089,22 +19083,22 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="0">
+      <c r="A44" s="39">
         <v>1424</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="0">
+      <c r="C44" s="39">
         <v>910530</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="0">
+      <c r="E44" s="39">
         <v>9.9</v>
       </c>
-      <c r="F44" s="0">
+      <c r="F44" s="40">
         <v>39.6</v>
       </c>
       <c r="G44" s="0">
@@ -19116,22 +19110,22 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="0">
+      <c r="A45" s="39">
         <v>1424</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="0">
+      <c r="C45" s="39">
         <v>910560</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="0">
+      <c r="E45" s="39">
         <v>7.5</v>
       </c>
-      <c r="F45" s="0">
+      <c r="F45" s="40">
         <v>30</v>
       </c>
       <c r="G45" s="0">
@@ -19143,22 +19137,22 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="0">
+      <c r="A46" s="39">
         <v>1424</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="0">
+      <c r="C46" s="39">
         <v>910810</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="0">
+      <c r="E46" s="39">
         <v>11.14</v>
       </c>
-      <c r="F46" s="0">
+      <c r="F46" s="40">
         <v>138.572</v>
       </c>
       <c r="G46" s="0">
@@ -19170,22 +19164,22 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="0">
+      <c r="A47" s="39">
         <v>1424</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="0">
+      <c r="C47" s="39">
         <v>910890</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="0">
+      <c r="E47" s="39">
         <v>1</v>
       </c>
-      <c r="F47" s="0">
+      <c r="F47" s="40">
         <v>13</v>
       </c>
       <c r="G47" s="0">
@@ -19197,22 +19191,22 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="0">
+      <c r="A48" s="39">
         <v>1424</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="0">
+      <c r="C48" s="39">
         <v>910920</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="0">
+      <c r="E48" s="39">
         <v>2.18</v>
       </c>
-      <c r="F48" s="0">
+      <c r="F48" s="40">
         <v>23.838</v>
       </c>
       <c r="G48" s="0">
@@ -19224,22 +19218,22 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="0">
+      <c r="A49" s="39">
         <v>1424</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="0">
+      <c r="C49" s="39">
         <v>910940</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="0">
+      <c r="E49" s="39">
         <v>1</v>
       </c>
-      <c r="F49" s="0">
+      <c r="F49" s="40">
         <v>13</v>
       </c>
       <c r="G49" s="0">
@@ -19251,22 +19245,22 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="0">
+      <c r="A50" s="39">
         <v>1424</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C50" s="0">
+      <c r="C50" s="39">
         <v>911250</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="0">
+      <c r="E50" s="39">
         <v>44.25</v>
       </c>
-      <c r="F50" s="0">
+      <c r="F50" s="40">
         <v>486.873</v>
       </c>
       <c r="G50" s="0">
@@ -19278,22 +19272,22 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="0">
+      <c r="A51" s="39">
         <v>1424</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="0">
+      <c r="C51" s="39">
         <v>913930</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="E51" s="0">
+      <c r="E51" s="39">
         <v>0</v>
       </c>
-      <c r="F51" s="0">
+      <c r="F51" s="40">
         <v>0</v>
       </c>
       <c r="G51" s="0">
@@ -19305,22 +19299,22 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="0">
+      <c r="A52" s="39">
         <v>1424</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="0">
+      <c r="C52" s="39">
         <v>914760</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="E52" s="0">
+      <c r="E52" s="39">
         <v>2.5</v>
       </c>
-      <c r="F52" s="0">
+      <c r="F52" s="40">
         <v>37.34</v>
       </c>
       <c r="G52" s="0">
@@ -19332,22 +19326,22 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="0">
+      <c r="A53" s="39">
         <v>1424</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="0">
+      <c r="C53" s="39">
         <v>914780</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="E53" s="0">
+      <c r="E53" s="39">
         <v>0.45</v>
       </c>
-      <c r="F53" s="0">
+      <c r="F53" s="40">
         <v>2.73</v>
       </c>
       <c r="G53" s="0">
@@ -19359,22 +19353,22 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="0">
+      <c r="A54" s="39">
         <v>1424</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="0">
+      <c r="C54" s="39">
         <v>920830</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E54" s="0">
+      <c r="E54" s="39">
         <v>0.4</v>
       </c>
-      <c r="F54" s="0">
+      <c r="F54" s="40">
         <v>2.4</v>
       </c>
       <c r="G54" s="0">
@@ -19386,22 +19380,22 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="0">
+      <c r="A55" s="39">
         <v>1424</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="0">
+      <c r="C55" s="39">
         <v>920850</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="E55" s="0">
+      <c r="E55" s="39">
         <v>5</v>
       </c>
-      <c r="F55" s="0">
+      <c r="F55" s="40">
         <v>15</v>
       </c>
       <c r="G55" s="0">
@@ -19413,22 +19407,22 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="0">
+      <c r="A56" s="39">
         <v>1424</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="0">
+      <c r="C56" s="39">
         <v>921010</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E56" s="0">
+      <c r="E56" s="39">
         <v>2.2</v>
       </c>
-      <c r="F56" s="0">
+      <c r="F56" s="40">
         <v>11</v>
       </c>
       <c r="G56" s="0">
@@ -19440,22 +19434,22 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="0">
+      <c r="A57" s="39">
         <v>1424</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="0">
+      <c r="C57" s="39">
         <v>921050</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="0">
+      <c r="E57" s="39">
         <v>6</v>
       </c>
-      <c r="F57" s="0">
+      <c r="F57" s="40">
         <v>30</v>
       </c>
       <c r="G57" s="0">
@@ -19467,22 +19461,22 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="0">
+      <c r="A58" s="39">
         <v>1424</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="0">
+      <c r="C58" s="39">
         <v>921060</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="E58" s="0">
+      <c r="E58" s="39">
         <v>47</v>
       </c>
-      <c r="F58" s="0">
+      <c r="F58" s="40">
         <v>235</v>
       </c>
       <c r="G58" s="0">
@@ -19494,22 +19488,22 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="0">
+      <c r="A59" s="39">
         <v>1424</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="0">
+      <c r="C59" s="39">
         <v>921070</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="E59" s="0">
+      <c r="E59" s="39">
         <v>2.2</v>
       </c>
-      <c r="F59" s="0">
+      <c r="F59" s="40">
         <v>11</v>
       </c>
       <c r="G59" s="0">
@@ -19521,22 +19515,22 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="0">
+      <c r="A60" s="39">
         <v>1424</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="0">
+      <c r="C60" s="39">
         <v>921080</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="0">
+      <c r="E60" s="39">
         <v>3</v>
       </c>
-      <c r="F60" s="0">
+      <c r="F60" s="40">
         <v>15</v>
       </c>
       <c r="G60" s="0">
@@ -19548,22 +19542,22 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="0">
+      <c r="A61" s="39">
         <v>1424</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="0">
+      <c r="C61" s="39">
         <v>921120</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="E61" s="0">
+      <c r="E61" s="39">
         <v>33</v>
       </c>
-      <c r="F61" s="0">
+      <c r="F61" s="40">
         <v>159.2</v>
       </c>
       <c r="G61" s="0">
@@ -19575,22 +19569,22 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="0">
+      <c r="A62" s="39">
         <v>1424</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="0">
+      <c r="C62" s="39">
         <v>921190</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E62" s="0">
+      <c r="E62" s="39">
         <v>1</v>
       </c>
-      <c r="F62" s="0">
+      <c r="F62" s="40">
         <v>4.6</v>
       </c>
       <c r="G62" s="0">
@@ -19602,22 +19596,22 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="0">
+      <c r="A63" s="39">
         <v>1424</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C63" s="0">
+      <c r="C63" s="39">
         <v>921500</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="0">
+      <c r="E63" s="39">
         <v>1.33</v>
       </c>
-      <c r="F63" s="0">
+      <c r="F63" s="40">
         <v>6.668</v>
       </c>
       <c r="G63" s="0">
@@ -19629,22 +19623,22 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="0">
+      <c r="A64" s="39">
         <v>1424</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="0">
+      <c r="C64" s="39">
         <v>921700</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="E64" s="0">
+      <c r="E64" s="39">
         <v>148</v>
       </c>
-      <c r="F64" s="0">
+      <c r="F64" s="40">
         <v>1409.8</v>
       </c>
       <c r="G64" s="0">
@@ -19656,22 +19650,22 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="0">
+      <c r="A65" s="39">
         <v>1424</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="0">
+      <c r="C65" s="39">
         <v>921910</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E65" s="0">
+      <c r="E65" s="39">
         <v>8.5</v>
       </c>
-      <c r="F65" s="0">
+      <c r="F65" s="40">
         <v>40.2</v>
       </c>
       <c r="G65" s="0">
@@ -19683,22 +19677,22 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="0">
+      <c r="A66" s="39">
         <v>1424</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="0">
+      <c r="C66" s="39">
         <v>921930</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="E66" s="0">
+      <c r="E66" s="39">
         <v>7.29</v>
       </c>
-      <c r="F66" s="0">
+      <c r="F66" s="40">
         <v>72.858</v>
       </c>
       <c r="G66" s="0">
@@ -19710,22 +19704,22 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="0">
+      <c r="A67" s="39">
         <v>1424</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C67" s="0">
+      <c r="C67" s="39">
         <v>922020</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="E67" s="0">
+      <c r="E67" s="39">
         <v>6</v>
       </c>
-      <c r="F67" s="0">
+      <c r="F67" s="40">
         <v>30</v>
       </c>
       <c r="G67" s="0">
@@ -19737,22 +19731,22 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="0">
+      <c r="A68" s="39">
         <v>1424</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C68" s="0">
+      <c r="C68" s="39">
         <v>922050</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="E68" s="0">
+      <c r="E68" s="39">
         <v>2</v>
       </c>
-      <c r="F68" s="0">
+      <c r="F68" s="40">
         <v>24</v>
       </c>
       <c r="G68" s="0">
@@ -19764,22 +19758,22 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="0">
+      <c r="A69" s="39">
         <v>1424</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="0">
+      <c r="C69" s="39">
         <v>922080</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="0">
+      <c r="E69" s="39">
         <v>12</v>
       </c>
-      <c r="F69" s="0">
+      <c r="F69" s="40">
         <v>120</v>
       </c>
       <c r="G69" s="0">
@@ -19791,22 +19785,22 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="0">
+      <c r="A70" s="39">
         <v>1424</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="0">
+      <c r="C70" s="39">
         <v>922300</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E70" s="0">
+      <c r="E70" s="39">
         <v>5.44</v>
       </c>
-      <c r="F70" s="0">
+      <c r="F70" s="40">
         <v>27.128</v>
       </c>
       <c r="G70" s="0">
@@ -19818,22 +19812,22 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="0">
+      <c r="A71" s="39">
         <v>1424</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="0">
+      <c r="C71" s="39">
         <v>922800</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="E71" s="0">
+      <c r="E71" s="39">
         <v>10</v>
       </c>
-      <c r="F71" s="0">
+      <c r="F71" s="40">
         <v>100</v>
       </c>
       <c r="G71" s="0">
@@ -19845,22 +19839,22 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="0">
+      <c r="A72" s="39">
         <v>1424</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="0">
+      <c r="C72" s="39">
         <v>922820</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E72" s="0">
+      <c r="E72" s="39">
         <v>2</v>
       </c>
-      <c r="F72" s="0">
+      <c r="F72" s="40">
         <v>20</v>
       </c>
       <c r="G72" s="0">
@@ -19872,22 +19866,22 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="0">
+      <c r="A73" s="39">
         <v>1424</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="0">
+      <c r="C73" s="39">
         <v>924210</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="E73" s="0">
+      <c r="E73" s="39">
         <v>7.44</v>
       </c>
-      <c r="F73" s="0">
+      <c r="F73" s="40">
         <v>37.189</v>
       </c>
       <c r="G73" s="0">
@@ -19899,22 +19893,22 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="0">
+      <c r="A74" s="39">
         <v>1424</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C74" s="0">
+      <c r="C74" s="39">
         <v>924220</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="D74" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E74" s="0">
+      <c r="E74" s="39">
         <v>0.14</v>
       </c>
-      <c r="F74" s="0">
+      <c r="F74" s="40">
         <v>0.681</v>
       </c>
       <c r="G74" s="0">
@@ -19926,22 +19920,22 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="0">
+      <c r="A75" s="39">
         <v>1424</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C75" s="0">
+      <c r="C75" s="39">
         <v>924280</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="E75" s="0">
+      <c r="E75" s="39">
         <v>0.04</v>
       </c>
-      <c r="F75" s="0">
+      <c r="F75" s="40">
         <v>0.04</v>
       </c>
       <c r="G75" s="0">
@@ -19953,22 +19947,22 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="0">
+      <c r="A76" s="39">
         <v>1424</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C76" s="0">
+      <c r="C76" s="39">
         <v>924820</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="E76" s="0">
+      <c r="E76" s="39">
         <v>2</v>
       </c>
-      <c r="F76" s="0">
+      <c r="F76" s="40">
         <v>4</v>
       </c>
       <c r="G76" s="0">
@@ -19980,22 +19974,22 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="0">
+      <c r="A77" s="39">
         <v>1424</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="0">
+      <c r="C77" s="39">
         <v>925060</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E77" s="0">
-        <v>8</v>
-      </c>
-      <c r="F77" s="0">
+      <c r="E77" s="39">
+        <v>8</v>
+      </c>
+      <c r="F77" s="40">
         <v>8</v>
       </c>
       <c r="G77" s="0">
@@ -20007,22 +20001,22 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="0">
+      <c r="A78" s="39">
         <v>1424</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C78" s="0">
+      <c r="C78" s="39">
         <v>925400</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E78" s="0">
+      <c r="E78" s="39">
         <v>18</v>
       </c>
-      <c r="F78" s="0">
+      <c r="F78" s="40">
         <v>180</v>
       </c>
       <c r="G78" s="0">
@@ -20034,22 +20028,22 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="0">
+      <c r="A79" s="39">
         <v>1424</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C79" s="0">
+      <c r="C79" s="39">
         <v>925410</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E79" s="0">
+      <c r="E79" s="39">
         <v>39</v>
       </c>
-      <c r="F79" s="0">
+      <c r="F79" s="40">
         <v>195</v>
       </c>
       <c r="G79" s="0">
@@ -20061,22 +20055,22 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="0">
+      <c r="A80" s="39">
         <v>1424</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C80" s="0">
+      <c r="C80" s="39">
         <v>925710</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="E80" s="0">
+      <c r="E80" s="39">
         <v>1</v>
       </c>
-      <c r="F80" s="0">
+      <c r="F80" s="40">
         <v>1</v>
       </c>
       <c r="G80" s="0">
@@ -20088,22 +20082,22 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="0">
+      <c r="A81" s="39">
         <v>1424</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C81" s="0">
+      <c r="C81" s="39">
         <v>926100</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E81" s="0">
+      <c r="E81" s="39">
         <v>6</v>
       </c>
-      <c r="F81" s="0">
+      <c r="F81" s="40">
         <v>12</v>
       </c>
       <c r="G81" s="0">
@@ -20115,22 +20109,22 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="0">
+      <c r="A82" s="39">
         <v>1424</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C82" s="0">
+      <c r="C82" s="39">
         <v>926210</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E82" s="0">
+      <c r="E82" s="39">
         <v>36.8</v>
       </c>
-      <c r="F82" s="0">
+      <c r="F82" s="40">
         <v>92</v>
       </c>
       <c r="G82" s="0">
@@ -20142,22 +20136,22 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="0">
+      <c r="A83" s="39">
         <v>1424</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="0">
+      <c r="C83" s="39">
         <v>926230</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="E83" s="0">
+      <c r="E83" s="39">
         <v>14</v>
       </c>
-      <c r="F83" s="0">
+      <c r="F83" s="40">
         <v>21</v>
       </c>
       <c r="G83" s="0">
@@ -20169,22 +20163,22 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="0">
+      <c r="A84" s="39">
         <v>1424</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="0">
+      <c r="C84" s="39">
         <v>926270</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="D84" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E84" s="0">
+      <c r="E84" s="39">
         <v>1</v>
       </c>
-      <c r="F84" s="0">
+      <c r="F84" s="40">
         <v>2.5</v>
       </c>
       <c r="G84" s="0">
@@ -20196,22 +20190,22 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="0">
+      <c r="A85" s="39">
         <v>1424</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C85" s="0">
+      <c r="C85" s="39">
         <v>926340</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="E85" s="0">
+      <c r="E85" s="39">
         <v>6</v>
       </c>
-      <c r="F85" s="0">
+      <c r="F85" s="40">
         <v>6</v>
       </c>
       <c r="G85" s="0">
@@ -20223,22 +20217,22 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="0">
+      <c r="A86" s="39">
         <v>1424</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="0">
+      <c r="C86" s="39">
         <v>926600</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="E86" s="0">
+      <c r="E86" s="39">
         <v>7</v>
       </c>
-      <c r="F86" s="0">
+      <c r="F86" s="40">
         <v>33.6</v>
       </c>
       <c r="G86" s="0">
@@ -20250,22 +20244,22 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="0">
+      <c r="A87" s="39">
         <v>1424</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="0">
+      <c r="C87" s="39">
         <v>927100</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="E87" s="0">
+      <c r="E87" s="39">
         <v>19</v>
       </c>
-      <c r="F87" s="0">
+      <c r="F87" s="40">
         <v>160.4</v>
       </c>
       <c r="G87" s="0">
@@ -20277,22 +20271,22 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="0">
+      <c r="A88" s="39">
         <v>1424</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C88" s="0">
+      <c r="C88" s="39">
         <v>928700</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E88" s="0">
+      <c r="E88" s="39">
         <v>1.17</v>
       </c>
-      <c r="F88" s="0">
+      <c r="F88" s="40">
         <v>2.1</v>
       </c>
       <c r="G88" s="0">
@@ -20304,22 +20298,22 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="0">
+      <c r="A89" s="39">
         <v>1424</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C89" s="0">
+      <c r="C89" s="39">
         <v>928720</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="E89" s="0">
+      <c r="E89" s="39">
         <v>4</v>
       </c>
-      <c r="F89" s="0">
+      <c r="F89" s="40">
         <v>12</v>
       </c>
       <c r="G89" s="0">
@@ -20331,22 +20325,22 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="0">
+      <c r="A90" s="39">
         <v>1424</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C90" s="0">
+      <c r="C90" s="39">
         <v>928800</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="E90" s="0">
+      <c r="E90" s="39">
         <v>1</v>
       </c>
-      <c r="F90" s="0">
+      <c r="F90" s="40">
         <v>13</v>
       </c>
       <c r="G90" s="0">
@@ -20358,22 +20352,22 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="0">
+      <c r="A91" s="39">
         <v>1424</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C91" s="0">
+      <c r="C91" s="39">
         <v>928840</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="E91" s="0">
+      <c r="E91" s="39">
         <v>1</v>
       </c>
-      <c r="F91" s="0">
+      <c r="F91" s="40">
         <v>5</v>
       </c>
       <c r="G91" s="0">
@@ -20385,22 +20379,22 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="0">
+      <c r="A92" s="39">
         <v>1424</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C92" s="0">
+      <c r="C92" s="39">
         <v>929300</v>
       </c>
-      <c r="D92" s="0" t="s">
+      <c r="D92" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="E92" s="0">
+      <c r="E92" s="39">
         <v>16.6</v>
       </c>
-      <c r="F92" s="0">
+      <c r="F92" s="40">
         <v>166</v>
       </c>
       <c r="G92" s="0">
@@ -20412,22 +20406,22 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="0">
+      <c r="A93" s="39">
         <v>1424</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C93" s="0">
+      <c r="C93" s="39">
         <v>929700</v>
       </c>
-      <c r="D93" s="0" t="s">
+      <c r="D93" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="E93" s="0">
+      <c r="E93" s="39">
         <v>1.25</v>
       </c>
-      <c r="F93" s="0">
+      <c r="F93" s="40">
         <v>10.5</v>
       </c>
       <c r="G93" s="0">
@@ -20439,22 +20433,22 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="0">
+      <c r="A94" s="39">
         <v>1424</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C94" s="0">
+      <c r="C94" s="39">
         <v>932500</v>
       </c>
-      <c r="D94" s="0" t="s">
+      <c r="D94" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="E94" s="0">
+      <c r="E94" s="39">
         <v>16.05</v>
       </c>
-      <c r="F94" s="0">
+      <c r="F94" s="40">
         <v>160.5</v>
       </c>
       <c r="G94" s="0">
@@ -20466,22 +20460,22 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="0">
+      <c r="A95" s="39">
         <v>1424</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="0">
+      <c r="C95" s="39">
         <v>932560</v>
       </c>
-      <c r="D95" s="0" t="s">
+      <c r="D95" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="E95" s="0">
+      <c r="E95" s="39">
         <v>48</v>
       </c>
-      <c r="F95" s="0">
+      <c r="F95" s="40">
         <v>480</v>
       </c>
       <c r="G95" s="0">
@@ -20493,22 +20487,22 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="0">
+      <c r="A96" s="39">
         <v>1424</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C96" s="0">
+      <c r="C96" s="39">
         <v>933430</v>
       </c>
-      <c r="D96" s="0" t="s">
+      <c r="D96" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="E96" s="0">
+      <c r="E96" s="39">
         <v>374.89</v>
       </c>
-      <c r="F96" s="0">
+      <c r="F96" s="40">
         <v>1874.47</v>
       </c>
       <c r="G96" s="0">
@@ -20520,22 +20514,22 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="0">
+      <c r="A97" s="39">
         <v>1424</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C97" s="0">
+      <c r="C97" s="39">
         <v>933450</v>
       </c>
-      <c r="D97" s="0" t="s">
+      <c r="D97" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="E97" s="0">
+      <c r="E97" s="39">
         <v>246</v>
       </c>
-      <c r="F97" s="0">
+      <c r="F97" s="40">
         <v>1230</v>
       </c>
       <c r="G97" s="0">
@@ -20547,22 +20541,22 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="0">
+      <c r="A98" s="39">
         <v>1424</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C98" s="0">
+      <c r="C98" s="39">
         <v>933550</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="D98" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="E98" s="0">
+      <c r="E98" s="39">
         <v>162</v>
       </c>
-      <c r="F98" s="0">
+      <c r="F98" s="40">
         <v>810</v>
       </c>
       <c r="G98" s="0">
@@ -20574,22 +20568,22 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="0">
+      <c r="A99" s="39">
         <v>1424</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C99" s="0">
+      <c r="C99" s="39">
         <v>933800</v>
       </c>
-      <c r="D99" s="0" t="s">
+      <c r="D99" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="E99" s="0">
+      <c r="E99" s="39">
         <v>61</v>
       </c>
-      <c r="F99" s="0">
+      <c r="F99" s="40">
         <v>610</v>
       </c>
       <c r="G99" s="0">
@@ -20601,22 +20595,22 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="0">
+      <c r="A100" s="39">
         <v>1424</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C100" s="0">
+      <c r="C100" s="39">
         <v>933830</v>
       </c>
-      <c r="D100" s="0" t="s">
+      <c r="D100" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="E100" s="0">
+      <c r="E100" s="39">
         <v>0.6</v>
       </c>
-      <c r="F100" s="0">
+      <c r="F100" s="40">
         <v>3</v>
       </c>
       <c r="G100" s="0">
@@ -20628,22 +20622,22 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="0">
+      <c r="A101" s="39">
         <v>1424</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="0">
+      <c r="C101" s="39">
         <v>935100</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="E101" s="0">
+      <c r="E101" s="39">
         <v>20</v>
       </c>
-      <c r="F101" s="0">
+      <c r="F101" s="40">
         <v>200</v>
       </c>
       <c r="G101" s="0">
@@ -20655,22 +20649,22 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="0">
+      <c r="A102" s="39">
         <v>1424</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C102" s="0">
+      <c r="C102" s="39">
         <v>945600</v>
       </c>
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="E102" s="0">
+      <c r="E102" s="39">
         <v>4</v>
       </c>
-      <c r="F102" s="0">
+      <c r="F102" s="40">
         <v>24</v>
       </c>
       <c r="G102" s="0">
@@ -20682,22 +20676,22 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="0">
+      <c r="A103" s="39">
         <v>1424</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C103" s="0">
+      <c r="C103" s="39">
         <v>974410</v>
       </c>
-      <c r="D103" s="0" t="s">
+      <c r="D103" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E103" s="0">
+      <c r="E103" s="39">
         <v>1</v>
       </c>
-      <c r="F103" s="0">
+      <c r="F103" s="40">
         <v>0.1</v>
       </c>
       <c r="G103" s="0">
@@ -20709,22 +20703,22 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="0">
+      <c r="A104" s="39">
         <v>1424</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C104" s="0">
+      <c r="C104" s="39">
         <v>977500</v>
       </c>
-      <c r="D104" s="0" t="s">
+      <c r="D104" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="E104" s="0">
+      <c r="E104" s="39">
         <v>2</v>
       </c>
-      <c r="F104" s="0">
+      <c r="F104" s="40">
         <v>2</v>
       </c>
       <c r="G104" s="0">

</xml_diff>